<commit_message>
final addition of data and removal of csv
</commit_message>
<xml_diff>
--- a/Data/confinement_thindouble_5.xlsx
+++ b/Data/confinement_thindouble_5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Google Drive\l'X\Stage LadHyX\Data\Time-Radius\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9834EBDB-C654-493B-B0B2-22BCEDD66E6C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CCEC7E0-1937-4DAD-AC2D-217A9A0847E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="420" yWindow="1884" windowWidth="17256" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="confinement_thindouble_5" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -2108,8 +2110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>